<commit_message>
added candidate in TestImageInfo
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cipleu\Documents\IULIA\SCOALA\facultate\Year 4 Semester 1\PRS\Lab\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A613FAA-24E7-47B6-AC24-43659C51A2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37DC2E7-D394-44E4-A825-E1A3EC0807FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C868631A-3BFC-4968-8E22-72B717EAB2D7}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{C868631A-3BFC-4968-8E22-72B717EAB2D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$G$1:$G$121</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="270">
   <si>
     <t>Image Name</t>
   </si>
@@ -55,9 +58,6 @@
     <t>WOR516K</t>
   </si>
   <si>
-    <t>21-801-27</t>
-  </si>
-  <si>
     <t>B81JKY</t>
   </si>
   <si>
@@ -67,9 +67,6 @@
     <t>VI47JAR</t>
   </si>
   <si>
-    <t>60-70?</t>
-  </si>
-  <si>
     <t>01CC1A0001</t>
   </si>
   <si>
@@ -145,15 +142,6 @@
     <t>Obs</t>
   </si>
   <si>
-    <t>see condition for valid candidates</t>
-  </si>
-  <si>
-    <t>41-RS-TZ</t>
-  </si>
-  <si>
-    <t>cannot see letters after binarization</t>
-  </si>
-  <si>
     <t>64-3185-44</t>
   </si>
   <si>
@@ -238,9 +226,6 @@
     <t>BMWM5</t>
   </si>
   <si>
-    <t>finds letters, but white on black</t>
-  </si>
-  <si>
     <t>BRIT0001</t>
   </si>
   <si>
@@ -337,9 +322,6 @@
     <t>FAMU2010</t>
   </si>
   <si>
-    <t>FASTVIRGINIA</t>
-  </si>
-  <si>
     <t>FI</t>
   </si>
   <si>
@@ -616,9 +598,6 @@
     <t>ORINNIE</t>
   </si>
   <si>
-    <t>OS802-HN</t>
-  </si>
-  <si>
     <t>OVI4VLL</t>
   </si>
   <si>
@@ -637,9 +616,6 @@
     <t>PEN15</t>
   </si>
   <si>
-    <t>maybe if inverted</t>
-  </si>
-  <si>
     <t>PGMN112</t>
   </si>
   <si>
@@ -751,9 +727,6 @@
     <t>UI5474</t>
   </si>
   <si>
-    <t>half of plate is not valid candidate</t>
-  </si>
-  <si>
     <t>UKC0917</t>
   </si>
   <si>
@@ -790,9 +763,6 @@
     <t>WIW123</t>
   </si>
   <si>
-    <t>WMY-9051</t>
-  </si>
-  <si>
     <t>WW95550</t>
   </si>
   <si>
@@ -811,13 +781,64 @@
     <t>YSX213</t>
   </si>
   <si>
-    <t>maybe if inverted, see condition for valid candidates</t>
-  </si>
-  <si>
-    <t>ZBO64MF-90-00</t>
-  </si>
-  <si>
     <t>ZENDOG</t>
+  </si>
+  <si>
+    <t>see condition for valid candidates: solved</t>
+  </si>
+  <si>
+    <t>see condition for valid candidates: thin letters</t>
+  </si>
+  <si>
+    <t>cannot segment characters</t>
+  </si>
+  <si>
+    <t>FAST</t>
+  </si>
+  <si>
+    <t>OS802HN</t>
+  </si>
+  <si>
+    <t>solved, by inverting and no candidate condition</t>
+  </si>
+  <si>
+    <t>half of plate is not valid candidate: solved</t>
+  </si>
+  <si>
+    <t>WMY9051</t>
+  </si>
+  <si>
+    <t>41RSTZ</t>
+  </si>
+  <si>
+    <t>ZBO64MF9000</t>
+  </si>
+  <si>
+    <t>cannot see letters after binarization: solved</t>
+  </si>
+  <si>
+    <t>maybe if inverted: solved</t>
+  </si>
+  <si>
+    <t>finds letters, but white on black: solved</t>
+  </si>
+  <si>
+    <t>CJ21RNA</t>
+  </si>
+  <si>
+    <t>CJ76KEM</t>
+  </si>
+  <si>
+    <t>SJ68YES</t>
+  </si>
+  <si>
+    <t>SJ99RBI</t>
+  </si>
+  <si>
+    <t>BH033314</t>
+  </si>
+  <si>
+    <t>SJ27YES</t>
   </si>
 </sst>
 </file>
@@ -874,8 +895,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8F33FFC-85B6-42EB-811F-D4E10156F5CE}" name="Table1" displayName="Table1" ref="A1:B125" totalsRowShown="0">
-  <autoFilter ref="A1:B125" xr:uid="{E8F33FFC-85B6-42EB-811F-D4E10156F5CE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8F33FFC-85B6-42EB-811F-D4E10156F5CE}" name="Table1" displayName="Table1" ref="A1:B130" totalsRowShown="0">
+  <autoFilter ref="A1:B130" xr:uid="{E8F33FFC-85B6-42EB-811F-D4E10156F5CE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B126">
+    <sortCondition ref="A1:A126"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E85AA671-4EB1-4522-95E9-0849BA8109D4}" name="Image Name"/>
     <tableColumn id="2" xr3:uid="{E8E8395B-E04D-4BDD-84AD-44E4C9441E4F}" name="Reason of Deletion"/>
@@ -1181,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F74FEC-1670-447E-A86E-6BF072FC778D}">
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,13 +1237,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1227,7 +1251,7 @@
         <v>145</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -1236,13 +1260,13 @@
         <v>60</v>
       </c>
       <c r="E2">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1259,13 +1283,13 @@
         <v>50</v>
       </c>
       <c r="E3">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F3">
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1296,7 +1320,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1316,7 +1340,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1336,7 +1360,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1348,18 +1372,18 @@
         <v>80</v>
       </c>
       <c r="E8">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F8">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
+      <c r="A9">
+        <v>218027</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1373,13 +1397,16 @@
       <c r="E9">
         <v>68</v>
       </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1399,7 +1426,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>259</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1417,7 +1444,7 @@
         <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1433,105 +1460,105 @@
       <c r="D12">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
-        <v>13</v>
+      <c r="E12">
+        <v>68</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D13">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E13">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="F13">
         <v>20</v>
-      </c>
-      <c r="G13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D14">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="E14">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F14">
         <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D15">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E15">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F15">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D16">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E16">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F16">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>40</v>
@@ -1545,10 +1572,13 @@
       <c r="F17">
         <v>20</v>
       </c>
+      <c r="G17" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1566,12 +1596,12 @@
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1588,13 +1618,10 @@
       <c r="F19">
         <v>20</v>
       </c>
-      <c r="G19" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1606,27 +1633,27 @@
         <v>60</v>
       </c>
       <c r="E20">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F20">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D21">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E21">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F21">
         <v>15</v>
@@ -1634,67 +1661,70 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E22">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F22">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
         <v>50</v>
       </c>
-      <c r="E23">
-        <v>90</v>
-      </c>
       <c r="F23">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E24">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1712,15 +1742,15 @@
         <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>39</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>40</v>
@@ -1735,15 +1765,15 @@
         <v>20</v>
       </c>
       <c r="G26" t="s">
-        <v>70</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C27">
         <v>40</v>
@@ -1758,12 +1788,12 @@
         <v>20</v>
       </c>
       <c r="G27" t="s">
-        <v>39</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>217</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1775,18 +1805,15 @@
         <v>60</v>
       </c>
       <c r="E28">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="F28">
-        <v>20</v>
-      </c>
-      <c r="G28" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1798,21 +1825,24 @@
         <v>60</v>
       </c>
       <c r="E29">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="F29">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="G29" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D30">
         <v>60</v>
@@ -1823,33 +1853,33 @@
       <c r="F30">
         <v>20</v>
       </c>
-      <c r="G30" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D31">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E31">
         <v>85</v>
       </c>
       <c r="F31">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="G31" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1866,25 +1896,22 @@
       <c r="F32">
         <v>20</v>
       </c>
-      <c r="G32" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D33">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E33">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F33">
         <v>20</v>
@@ -1892,36 +1919,39 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C34">
         <v>40</v>
       </c>
       <c r="D34">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E34">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F34">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="G34" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D35">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E35">
         <v>85</v>
@@ -1929,13 +1959,10 @@
       <c r="F35">
         <v>20</v>
       </c>
-      <c r="G35" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1947,15 +1974,18 @@
         <v>60</v>
       </c>
       <c r="E36">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F36">
         <v>20</v>
+      </c>
+      <c r="G36" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1970,21 +2000,18 @@
         <v>85</v>
       </c>
       <c r="F37">
-        <v>20</v>
-      </c>
-      <c r="G37" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D38">
         <v>60</v>
@@ -1993,12 +2020,12 @@
         <v>85</v>
       </c>
       <c r="F38">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2018,118 +2045,121 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="D40">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E40">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F40">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G40" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>20</v>
-      </c>
-      <c r="D41">
-        <v>20</v>
-      </c>
-      <c r="E41">
-        <v>85</v>
-      </c>
-      <c r="F41">
-        <v>20</v>
-      </c>
-      <c r="G41" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>237</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>90</v>
+      </c>
+      <c r="F42">
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>247</v>
+        <v>94</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C43">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D43">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E43">
         <v>90</v>
       </c>
       <c r="F43">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D44">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="E44">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F44">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G44" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>254</v>
       </c>
       <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>15</v>
+      </c>
+      <c r="E45">
+        <v>95</v>
+      </c>
+      <c r="F45">
         <v>5</v>
       </c>
-      <c r="C45">
-        <v>40</v>
-      </c>
-      <c r="D45">
-        <v>60</v>
-      </c>
-      <c r="E45">
-        <v>90</v>
-      </c>
-      <c r="F45">
-        <v>20</v>
+      <c r="G45" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -2141,81 +2171,75 @@
         <v>15</v>
       </c>
       <c r="E46">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F46">
-        <v>20</v>
-      </c>
-      <c r="G46" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C47">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D47">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E47">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="F47">
-        <v>20</v>
-      </c>
-      <c r="G47" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D48">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="E48">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F48">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D49">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E49">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="F49">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2227,7 +2251,7 @@
         <v>60</v>
       </c>
       <c r="E50">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F50">
         <v>20</v>
@@ -2235,10 +2259,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C51">
         <v>40</v>
@@ -2247,15 +2271,18 @@
         <v>60</v>
       </c>
       <c r="E51">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="F51">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2267,7 +2294,7 @@
         <v>60</v>
       </c>
       <c r="E52">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="F52">
         <v>20</v>
@@ -2275,7 +2302,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2292,13 +2319,10 @@
       <c r="F53">
         <v>20</v>
       </c>
-      <c r="G53" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2310,7 +2334,7 @@
         <v>60</v>
       </c>
       <c r="E54">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F54">
         <v>20</v>
@@ -2318,10 +2342,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55">
         <v>40</v>
@@ -2330,7 +2354,7 @@
         <v>60</v>
       </c>
       <c r="E55">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F55">
         <v>20</v>
@@ -2341,7 +2365,7 @@
         <v>122</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56">
         <v>40</v>
@@ -2350,7 +2374,7 @@
         <v>60</v>
       </c>
       <c r="E56">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="F56">
         <v>20</v>
@@ -2358,10 +2382,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C57">
         <v>40</v>
@@ -2370,7 +2394,7 @@
         <v>60</v>
       </c>
       <c r="E57">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="F57">
         <v>20</v>
@@ -2378,19 +2402,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D58">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E58">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="F58">
         <v>20</v>
@@ -2398,10 +2422,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C59">
         <v>40</v>
@@ -2410,27 +2434,27 @@
         <v>60</v>
       </c>
       <c r="E59">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F59">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D60">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E60">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F60">
         <v>20</v>
@@ -2441,7 +2465,7 @@
         <v>133</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C61">
         <v>40</v>
@@ -2450,18 +2474,18 @@
         <v>60</v>
       </c>
       <c r="E61">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="F61">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62">
         <v>40</v>
@@ -2470,7 +2494,7 @@
         <v>60</v>
       </c>
       <c r="E62">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="F62">
         <v>20</v>
@@ -2478,10 +2502,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B63">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C63">
         <v>40</v>
@@ -2490,7 +2514,7 @@
         <v>60</v>
       </c>
       <c r="E63">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="F63">
         <v>20</v>
@@ -2498,7 +2522,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2510,15 +2534,18 @@
         <v>60</v>
       </c>
       <c r="E64">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F64">
         <v>20</v>
+      </c>
+      <c r="G64" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2538,7 +2565,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2550,18 +2577,15 @@
         <v>60</v>
       </c>
       <c r="E66">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F66">
         <v>20</v>
-      </c>
-      <c r="G66" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2573,7 +2597,7 @@
         <v>60</v>
       </c>
       <c r="E67">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F67">
         <v>20</v>
@@ -2581,19 +2605,19 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C68">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D68">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E68">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F68">
         <v>20</v>
@@ -2601,36 +2625,36 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>149</v>
+        <v>10</v>
       </c>
       <c r="B69">
         <v>1</v>
       </c>
       <c r="C69">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D69">
         <v>60</v>
       </c>
       <c r="E69">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F69">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D70">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E70">
         <v>80</v>
@@ -2641,13 +2665,13 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>155</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C71">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D71">
         <v>60</v>
@@ -2656,12 +2680,12 @@
         <v>80</v>
       </c>
       <c r="F71">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2673,7 +2697,7 @@
         <v>60</v>
       </c>
       <c r="E72">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F72">
         <v>20</v>
@@ -2681,10 +2705,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C73">
         <v>40</v>
@@ -2701,7 +2725,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2713,7 +2737,7 @@
         <v>60</v>
       </c>
       <c r="E74">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F74">
         <v>20</v>
@@ -2721,7 +2745,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2741,10 +2765,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C76">
         <v>40</v>
@@ -2761,7 +2785,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2773,15 +2797,18 @@
         <v>60</v>
       </c>
       <c r="E77">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F77">
         <v>20</v>
+      </c>
+      <c r="G77" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B78">
         <v>3</v>
@@ -2796,15 +2823,15 @@
         <v>80</v>
       </c>
       <c r="F78">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C79">
         <v>40</v>
@@ -2816,18 +2843,15 @@
         <v>80</v>
       </c>
       <c r="F79">
-        <v>1</v>
-      </c>
-      <c r="G79" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B80">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C80">
         <v>40</v>
@@ -2839,12 +2863,12 @@
         <v>80</v>
       </c>
       <c r="F80">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -2856,24 +2880,24 @@
         <v>60</v>
       </c>
       <c r="E81">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F81">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C82">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D82">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E82">
         <v>80</v>
@@ -2884,10 +2908,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <v>40</v>
@@ -2896,24 +2920,24 @@
         <v>60</v>
       </c>
       <c r="E83">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F83">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B84">
         <v>1</v>
       </c>
       <c r="C84">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D84">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E84">
         <v>80</v>
@@ -2924,7 +2948,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2936,18 +2960,18 @@
         <v>60</v>
       </c>
       <c r="E85">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="F85">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C86">
         <v>40</v>
@@ -2964,56 +2988,62 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B87">
         <v>1</v>
       </c>
       <c r="C87">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D87">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E87">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F87">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="G87" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C88">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D88">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E88">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F88">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="G88" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>191</v>
+        <v>255</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D89">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E89">
         <v>80</v>
@@ -3022,38 +3052,38 @@
         <v>20</v>
       </c>
       <c r="G89" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="C90">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D90">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E90">
         <v>80</v>
       </c>
       <c r="F90">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G90" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C91">
         <v>40</v>
@@ -3062,13 +3092,10 @@
         <v>60</v>
       </c>
       <c r="E91">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="F91">
-        <v>20</v>
-      </c>
-      <c r="G91" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3076,22 +3103,19 @@
         <v>197</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C92">
         <v>40</v>
       </c>
       <c r="D92">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E92">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F92">
         <v>20</v>
-      </c>
-      <c r="G92" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3099,7 +3123,7 @@
         <v>199</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C93">
         <v>40</v>
@@ -3108,18 +3132,21 @@
         <v>60</v>
       </c>
       <c r="E93">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="F93">
         <v>15</v>
       </c>
+      <c r="G93" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94">
         <v>40</v>
@@ -3128,30 +3155,27 @@
         <v>60</v>
       </c>
       <c r="E94">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F94">
-        <v>5</v>
-      </c>
-      <c r="G94" t="s">
-        <v>203</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B95">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C95">
         <v>40</v>
       </c>
       <c r="D95">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E95">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="F95">
         <v>20</v>
@@ -3159,53 +3183,53 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B96">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C96">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D96">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E96">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F96">
-        <v>20</v>
-      </c>
-      <c r="G96" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D97">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E97">
         <v>85</v>
       </c>
       <c r="F97">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G97" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98">
         <v>40</v>
@@ -3214,67 +3238,67 @@
         <v>60</v>
       </c>
       <c r="E98">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="F98">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>212</v>
+        <v>17</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C99">
         <v>40</v>
       </c>
       <c r="D99">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E99">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="F99">
-        <v>20</v>
-      </c>
-      <c r="G99" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B100">
         <v>1</v>
       </c>
       <c r="C100">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D100">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E100">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F100">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="G100" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D101">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E101">
         <v>80</v>
@@ -3282,13 +3306,10 @@
       <c r="F101">
         <v>20</v>
       </c>
-      <c r="G101" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -3300,7 +3321,7 @@
         <v>60</v>
       </c>
       <c r="E102">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F102">
         <v>10</v>
@@ -3308,70 +3329,70 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>19</v>
+        <v>221</v>
       </c>
       <c r="B103">
         <v>1</v>
       </c>
       <c r="C103">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D103">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E103">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="F103">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B104">
         <v>1</v>
       </c>
       <c r="C104">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D104">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E104">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F104">
-        <v>20</v>
-      </c>
-      <c r="G104" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C105">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D105">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E105">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="F105">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="G105" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -3383,27 +3404,30 @@
         <v>60</v>
       </c>
       <c r="E106">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="F106">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G106" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
       <c r="C107">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D107">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E107">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="F107">
         <v>20</v>
@@ -3411,19 +3435,19 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B108">
         <v>1</v>
       </c>
       <c r="C108">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D108">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E108">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F108">
         <v>15</v>
@@ -3431,24 +3455,30 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C109">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D109">
-        <v>10</v>
+        <v>60</v>
+      </c>
+      <c r="E109">
+        <v>80</v>
+      </c>
+      <c r="F109">
+        <v>20</v>
       </c>
       <c r="G109" t="s">
-        <v>39</v>
+        <v>257</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -3460,21 +3490,18 @@
         <v>60</v>
       </c>
       <c r="E110">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F110">
         <v>20</v>
-      </c>
-      <c r="G110" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C111">
         <v>40</v>
@@ -3483,21 +3510,24 @@
         <v>60</v>
       </c>
       <c r="E111">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F111">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="G111" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C112">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D112">
         <v>60</v>
@@ -3506,21 +3536,24 @@
         <v>90</v>
       </c>
       <c r="F112">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="G112" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>240</v>
+        <v>11</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C113">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="D113">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E113">
         <v>80</v>
@@ -3528,13 +3561,10 @@
       <c r="F113">
         <v>20</v>
       </c>
-      <c r="G113" t="s">
-        <v>241</v>
-      </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -3546,81 +3576,84 @@
         <v>60</v>
       </c>
       <c r="E114">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F114">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="G114" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B115">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C115">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D115">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E115">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="F115">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G115" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="B116">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C116">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D116">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E116">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="F116">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G116" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B117">
         <v>2</v>
       </c>
       <c r="C117">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D117">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E117">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F117">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -3632,72 +3665,78 @@
         <v>60</v>
       </c>
       <c r="E118">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F118">
-        <v>20</v>
-      </c>
-      <c r="G118" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="27.75" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>253</v>
+        <v>7</v>
       </c>
       <c r="B119">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C119">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D119">
-        <v>20</v>
-      </c>
-      <c r="G119" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="E119">
+        <v>90</v>
+      </c>
+      <c r="F119">
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B120">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C120">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D120">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="E120">
+        <v>85</v>
+      </c>
+      <c r="F120">
+        <v>10</v>
       </c>
       <c r="G120" t="s">
-        <v>39</v>
+        <v>263</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>8</v>
+        <v>250</v>
       </c>
       <c r="B121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C121">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D121">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E121">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F121">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -3717,10 +3756,10 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="B123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C123">
         <v>40</v>
@@ -3734,25 +3773,22 @@
       <c r="F123">
         <v>20</v>
       </c>
-      <c r="G123" t="s">
-        <v>261</v>
-      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>7</v>
+        <v>266</v>
       </c>
       <c r="B124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C124">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D124">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E124">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F124">
         <v>20</v>
@@ -3760,30 +3796,27 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="B125">
         <v>1</v>
       </c>
       <c r="C125">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D125">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E125">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F125">
-        <v>10</v>
-      </c>
-      <c r="G125" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -3795,15 +3828,36 @@
         <v>60</v>
       </c>
       <c r="E126">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="F126">
         <v>20</v>
       </c>
     </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>269</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127">
+        <v>40</v>
+      </c>
+      <c r="D127">
+        <v>60</v>
+      </c>
+      <c r="E127">
+        <v>55</v>
+      </c>
+      <c r="F127">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G126">
-    <sortCondition ref="A19:A126"/>
+  <autoFilter ref="G1:G121" xr:uid="{81F74FEC-1670-447E-A86E-6BF072FC778D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G121">
+    <sortCondition ref="A18:A121"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -3812,10 +3866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05994B51-2DA8-41EC-8C3A-0F8203EDE17D}">
-  <dimension ref="A1:B125"/>
+  <dimension ref="A1:B130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3825,92 +3879,92 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
+      <c r="A2">
+        <v>983</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
+      <c r="A3">
+        <v>9214</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -3918,906 +3972,946 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>983</v>
+      <c r="A16" t="s">
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>9214</v>
+      <c r="A17" t="s">
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B49" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B51" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B52" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B55" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B58" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B60" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B61" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B63" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B64" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B66" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B67" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B69" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B70" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B72" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B73" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B74" t="s">
-        <v>126</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B75" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B76" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B77" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B78" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B79" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B80" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B81" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B82" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B83" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B84" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B85" t="s">
-        <v>126</v>
+        <v>26</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="B86" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B87" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B88" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B89" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B90" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B91" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B92" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B93" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B94" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B95" t="s">
-        <v>126</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B96" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B97" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B98" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B99" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B100" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B101" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B102" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B103" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B104" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B105" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B106" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B107" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B108" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B109" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B110" t="s">
-        <v>34</v>
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="B111" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="B112" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B113" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B114" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B115" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B116" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="B117" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="B118" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B119" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="B120" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B121" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="B122" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="B123" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B124" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="B125" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>248</v>
+      </c>
+      <c r="B126" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>93</v>
+      </c>
+      <c r="B127" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>249</v>
+      </c>
+      <c r="B128" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>203</v>
+      </c>
+      <c r="B129" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>194</v>
+      </c>
+      <c r="B130" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>